<commit_message>
data points + report started
</commit_message>
<xml_diff>
--- a/lab10data.xlsx
+++ b/lab10data.xlsx
@@ -1,45 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olegglotov/Documents/MAC/Python/2XC3 - Pratice and Exp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emmaw\OneDrive\Documents\2XC3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E24805-B6A9-9649-BF50-DA3D20C1DCFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CDA5DF8-4111-46C1-B0BD-64ABAC6483E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16140" xr2:uid="{DC596DBC-0CF1-4040-B4CF-422978E20046}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DC596DBC-0CF1-4040-B4CF-422978E20046}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$O$6:$O$58</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$P$4</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$P$6:$P$61</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$Q$4</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$Q$6:$Q$58</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$R$4</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$R$6:$R$58</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$S$6:$S$58</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$O$6:$O$58</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$P$4</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Sheet1!$P$6:$P$61</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Sheet1!$Q$4</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$P$6:$P$61</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Sheet1!$Q$6:$Q$58</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">Sheet1!$R$4</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">Sheet1!$R$6:$R$58</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">Sheet1!$S$6:$S$58</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$Q$4</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$Q$6:$Q$58</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$R$4</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$R$6:$R$58</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$S$6:$S$58</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$O$6:$O$58</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$P$4</definedName>
     <definedName name="VC1approx_1" localSheetId="0">Sheet1!$C$5:$E$61</definedName>
     <definedName name="VC2approx" localSheetId="0">Sheet1!$G$5:$I$58</definedName>
     <definedName name="VC3approx" localSheetId="0">Sheet1!$K$5:$M$58</definedName>
@@ -66,7 +42,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{F9D0599B-DFE1-574A-92A5-5000445B043B}" name="VC1approx" type="6" refreshedVersion="7" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/olegglotov/Documents/MAC/Python/2XC3 - Pratice and Exp/VC1approx.csv" comma="1">
+    <textPr sourceFile="/Users/olegglotov/Documents/MAC/Python/2XC3 - Pratice and Exp/VC1approx.csv" comma="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -75,7 +51,7 @@
     </textPr>
   </connection>
   <connection id="2" xr16:uid="{B5D7A7A8-853B-6F4C-A0D3-C6C105A4B3DD}" name="VC2approx" type="6" refreshedVersion="7" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/olegglotov/Documents/MAC/Python/2XC3 - Pratice and Exp/VC2approx.csv" comma="1">
+    <textPr sourceFile="/Users/olegglotov/Documents/MAC/Python/2XC3 - Pratice and Exp/VC2approx.csv" comma="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -84,7 +60,7 @@
     </textPr>
   </connection>
   <connection id="3" xr16:uid="{A0520909-81CA-E447-BC79-40024126780D}" name="VC3approx" type="6" refreshedVersion="7" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/olegglotov/Documents/MAC/Python/2XC3 - Pratice and Exp/VC3approx.csv" comma="1">
+    <textPr sourceFile="/Users/olegglotov/Documents/MAC/Python/2XC3 - Pratice and Exp/VC3approx.csv" comma="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -118,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="11">
   <si>
     <t>input size</t>
   </si>
@@ -148,6 +124,9 @@
   </si>
   <si>
     <t>5 runs avg VC3</t>
+  </si>
+  <si>
+    <t>2*best approx</t>
   </si>
 </sst>
 </file>
@@ -302,7 +281,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$O$6:$O$58</c:f>
+              <c:f>Sheet1!$B$64:$B$116</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="53"/>
@@ -470,7 +449,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$S$6:$S$58</c:f>
+              <c:f>Sheet1!$F$64:$F$116</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="53"/>
@@ -648,7 +627,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$P$4</c:f>
+              <c:f>Sheet1!$C$62</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -671,7 +650,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$O$6:$O$58</c:f>
+              <c:f>Sheet1!$B$64:$B$116</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="53"/>
@@ -839,7 +818,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$6:$P$61</c:f>
+              <c:f>Sheet1!$C$64:$C$119</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="56"/>
@@ -874,10 +853,10 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>11.6</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12.4</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>11.7</c:v>
@@ -1026,7 +1005,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$Q$4</c:f>
+              <c:f>Sheet1!$D$62</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1049,7 +1028,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$O$6:$O$58</c:f>
+              <c:f>Sheet1!$B$64:$B$116</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="53"/>
@@ -1217,7 +1196,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Q$6:$Q$58</c:f>
+              <c:f>Sheet1!$D$64:$D$116</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="53"/>
@@ -1261,7 +1240,7 @@
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>15</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>15</c:v>
@@ -1395,7 +1374,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$R$4</c:f>
+              <c:f>Sheet1!$E$62</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1418,7 +1397,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$O$6:$O$58</c:f>
+              <c:f>Sheet1!$B$64:$B$116</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="53"/>
@@ -1586,7 +1565,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$R$6:$R$58</c:f>
+              <c:f>Sheet1!$E$64:$E$116</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="53"/>
@@ -1756,6 +1735,375 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-ECF8-D84B-BD14-2165DA897DAF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$62</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2*best approx</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$64:$B$116</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="53"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>166</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>226</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>286</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>316</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>346</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>376</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>406</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>466</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>496</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>526</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>556</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>586</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$64:$G$116</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="53"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>274</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>318</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>366</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>466</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>526</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>564</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>626</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>680</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>724</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>774</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>820</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>890</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>922</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>974</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-DC9F-4027-8331-45E285601BF8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2661,16 +3009,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>702733</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>169334</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>249383</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>762001</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>135467</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>742951</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>96981</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3007,29 +3355,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1667BE23-77CE-F645-AC81-A38283E226F2}">
-  <dimension ref="C3:S61"/>
+  <dimension ref="B3:T119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I2" zoomScale="75" workbookViewId="0">
-      <selection activeCell="S39" sqref="S39"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.296875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.296875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.296875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="13.69921875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>3</v>
       </c>
@@ -3040,7 +3388,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="3:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>0</v>
       </c>
@@ -3083,8 +3431,11 @@
       <c r="S4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="T4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C6">
         <v>2</v>
       </c>
@@ -3132,8 +3483,12 @@
         <f>MIN(E6:E61,I6:I58, M6:M58)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="T6">
+        <f>S6*2</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C7">
         <v>3</v>
       </c>
@@ -3162,7 +3517,7 @@
         <v>2</v>
       </c>
       <c r="O7">
-        <f t="shared" ref="O7:O61" si="0">C7</f>
+        <f t="shared" ref="O7:O58" si="0">C7</f>
         <v>3</v>
       </c>
       <c r="P7">
@@ -3175,11 +3530,15 @@
         <v>2</v>
       </c>
       <c r="S7">
-        <f t="shared" ref="S7:S39" si="1">MIN(E7:E62,I7:I59, M7:M59)</f>
+        <f t="shared" ref="S7:S38" si="1">MIN(E7:E62,I7:I59, M7:M59)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="T7">
+        <f t="shared" ref="T7:T58" si="2">S7*2</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C8">
         <v>4</v>
       </c>
@@ -3224,8 +3583,12 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="T8">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C9">
         <v>5</v>
       </c>
@@ -3268,10 +3631,14 @@
       </c>
       <c r="S9">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="3:19" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C10">
         <v>6</v>
       </c>
@@ -3314,10 +3681,14 @@
       </c>
       <c r="S10">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="3:19" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C11">
         <v>7</v>
       </c>
@@ -3360,10 +3731,14 @@
       </c>
       <c r="S11">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="3:19" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C12">
         <v>8</v>
       </c>
@@ -3406,10 +3781,14 @@
       </c>
       <c r="S12">
         <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="3:19" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C13">
         <v>9</v>
       </c>
@@ -3452,10 +3831,14 @@
       </c>
       <c r="S13">
         <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="3:19" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C14">
         <v>10</v>
       </c>
@@ -3498,10 +3881,14 @@
       </c>
       <c r="S14">
         <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="3:19" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C15">
         <v>11</v>
       </c>
@@ -3544,10 +3931,14 @@
       </c>
       <c r="S15">
         <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="3:19" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C16">
         <v>12</v>
       </c>
@@ -3590,10 +3981,14 @@
       </c>
       <c r="S16">
         <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="3:19" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C17">
         <v>13</v>
       </c>
@@ -3636,10 +4031,14 @@
       </c>
       <c r="S17">
         <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="3:19" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C18">
         <v>14</v>
       </c>
@@ -3682,10 +4081,14 @@
       </c>
       <c r="S18">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="3:19" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="T18">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C19">
         <v>15</v>
       </c>
@@ -3728,10 +4131,14 @@
       </c>
       <c r="S19">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="3:19" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="T19">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C20">
         <v>16</v>
       </c>
@@ -3774,10 +4181,14 @@
       </c>
       <c r="S20">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="3:19" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="T20">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C21">
         <v>17</v>
       </c>
@@ -3820,10 +4231,14 @@
       </c>
       <c r="S21">
         <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="3:19" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="T21">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C22">
         <v>18</v>
       </c>
@@ -3866,10 +4281,14 @@
       </c>
       <c r="S22">
         <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="3:19" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="T22">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C23">
         <v>19</v>
       </c>
@@ -3912,10 +4331,14 @@
       </c>
       <c r="S23">
         <f>MIN(E23:E78,I23:I75, M23:M75)</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="3:19" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="T23">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C24">
         <v>20</v>
       </c>
@@ -3958,10 +4381,14 @@
       </c>
       <c r="S24">
         <f>MIN(E24:E79,I24:I76, M24:M76)</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="3:19" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="T24">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C25">
         <v>21</v>
       </c>
@@ -4004,10 +4431,14 @@
       </c>
       <c r="S25">
         <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="3:19" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="T25">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C26">
         <v>26</v>
       </c>
@@ -4050,10 +4481,14 @@
       </c>
       <c r="S26">
         <f t="shared" si="1"/>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="3:19" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="T26">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C27">
         <v>31</v>
       </c>
@@ -4096,10 +4531,14 @@
       </c>
       <c r="S27">
         <f t="shared" si="1"/>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="3:19" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="T27">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C28">
         <v>36</v>
       </c>
@@ -4142,10 +4581,14 @@
       </c>
       <c r="S28">
         <f t="shared" si="1"/>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="3:19" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="T28">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C29">
         <v>41</v>
       </c>
@@ -4188,10 +4631,14 @@
       </c>
       <c r="S29">
         <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="30" spans="3:19" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="T29">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C30">
         <v>46</v>
       </c>
@@ -4234,10 +4681,14 @@
       </c>
       <c r="S30">
         <f t="shared" si="1"/>
-        <v>37</v>
-      </c>
-    </row>
-    <row r="31" spans="3:19" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="T30">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C31">
         <v>51</v>
       </c>
@@ -4280,10 +4731,14 @@
       </c>
       <c r="S31">
         <f t="shared" si="1"/>
-        <v>38</v>
-      </c>
-    </row>
-    <row r="32" spans="3:19" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C32">
         <v>56</v>
       </c>
@@ -4326,10 +4781,14 @@
       </c>
       <c r="S32">
         <f>MIN(E32:E87,I32:I84, M32:M84)</f>
-        <v>41</v>
-      </c>
-    </row>
-    <row r="33" spans="3:19" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="T32">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C33">
         <v>61</v>
       </c>
@@ -4372,10 +4831,14 @@
       </c>
       <c r="S33">
         <f t="shared" si="1"/>
-        <v>48</v>
-      </c>
-    </row>
-    <row r="34" spans="3:19" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="T33">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C34">
         <v>66</v>
       </c>
@@ -4418,10 +4881,14 @@
       </c>
       <c r="S34">
         <f t="shared" si="1"/>
-        <v>53</v>
-      </c>
-    </row>
-    <row r="35" spans="3:19" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="T34">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C35">
         <v>71</v>
       </c>
@@ -4464,10 +4931,14 @@
       </c>
       <c r="S35">
         <f t="shared" si="1"/>
-        <v>56</v>
-      </c>
-    </row>
-    <row r="36" spans="3:19" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="T35">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C36">
         <v>76</v>
       </c>
@@ -4510,10 +4981,14 @@
       </c>
       <c r="S36">
         <f t="shared" si="1"/>
-        <v>58</v>
-      </c>
-    </row>
-    <row r="37" spans="3:19" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="T36">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C37">
         <v>81</v>
       </c>
@@ -4556,10 +5031,14 @@
       </c>
       <c r="S37">
         <f t="shared" si="1"/>
-        <v>65</v>
-      </c>
-    </row>
-    <row r="38" spans="3:19" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="T37">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C38">
         <v>86</v>
       </c>
@@ -4602,10 +5081,14 @@
       </c>
       <c r="S38">
         <f t="shared" si="1"/>
-        <v>68</v>
-      </c>
-    </row>
-    <row r="39" spans="3:19" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="T38">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C39">
         <v>91</v>
       </c>
@@ -4648,10 +5131,14 @@
       </c>
       <c r="S39">
         <f>MIN(E39:E94,I39:I91, M39:M91)</f>
-        <v>73</v>
-      </c>
-    </row>
-    <row r="40" spans="3:19" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="T39">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C40">
         <v>96</v>
       </c>
@@ -4693,11 +5180,15 @@
         <v>76</v>
       </c>
       <c r="S40">
-        <f t="shared" ref="S40:S58" si="2">MIN(E40:E95,I40:I92, M40:M92)</f>
-        <v>75</v>
-      </c>
-    </row>
-    <row r="41" spans="3:19" x14ac:dyDescent="0.2">
+        <f t="shared" ref="S40:S58" si="3">MIN(E40:E95,I40:I92, M40:M92)</f>
+        <v>1</v>
+      </c>
+      <c r="T40">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C41">
         <v>101</v>
       </c>
@@ -4739,11 +5230,15 @@
         <v>84</v>
       </c>
       <c r="S41">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="T41">
         <f t="shared" si="2"/>
-        <v>81</v>
-      </c>
-    </row>
-    <row r="42" spans="3:19" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C42">
         <v>106</v>
       </c>
@@ -4785,11 +5280,15 @@
         <v>100</v>
       </c>
       <c r="S42">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="T42">
         <f t="shared" si="2"/>
-        <v>82</v>
-      </c>
-    </row>
-    <row r="43" spans="3:19" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C43">
         <v>136</v>
       </c>
@@ -4831,11 +5330,15 @@
         <v>118</v>
       </c>
       <c r="S43">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="T43">
         <f t="shared" si="2"/>
-        <v>108</v>
-      </c>
-    </row>
-    <row r="44" spans="3:19" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C44">
         <v>166</v>
       </c>
@@ -4877,11 +5380,15 @@
         <v>144</v>
       </c>
       <c r="S44">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="T44">
         <f t="shared" si="2"/>
-        <v>137</v>
-      </c>
-    </row>
-    <row r="45" spans="3:19" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C45">
         <v>196</v>
       </c>
@@ -4923,11 +5430,15 @@
         <v>168</v>
       </c>
       <c r="S45">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="T45">
         <f t="shared" si="2"/>
-        <v>159</v>
-      </c>
-    </row>
-    <row r="46" spans="3:19" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C46">
         <v>226</v>
       </c>
@@ -4969,11 +5480,15 @@
         <v>193</v>
       </c>
       <c r="S46">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="T46">
         <f t="shared" si="2"/>
-        <v>183</v>
-      </c>
-    </row>
-    <row r="47" spans="3:19" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C47">
         <v>256</v>
       </c>
@@ -5015,11 +5530,15 @@
         <v>237</v>
       </c>
       <c r="S47">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="T47">
         <f t="shared" si="2"/>
-        <v>205</v>
-      </c>
-    </row>
-    <row r="48" spans="3:19" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C48">
         <v>286</v>
       </c>
@@ -5061,11 +5580,15 @@
         <v>250</v>
       </c>
       <c r="S48">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="T48">
         <f t="shared" si="2"/>
-        <v>233</v>
-      </c>
-    </row>
-    <row r="49" spans="3:19" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C49">
         <v>316</v>
       </c>
@@ -5107,11 +5630,15 @@
         <v>286</v>
       </c>
       <c r="S49">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="T49">
         <f t="shared" si="2"/>
-        <v>263</v>
-      </c>
-    </row>
-    <row r="50" spans="3:19" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C50">
         <v>346</v>
       </c>
@@ -5153,11 +5680,15 @@
         <v>316</v>
       </c>
       <c r="S50">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="T50">
         <f t="shared" si="2"/>
-        <v>282</v>
-      </c>
-    </row>
-    <row r="51" spans="3:19" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C51">
         <v>376</v>
       </c>
@@ -5199,11 +5730,15 @@
         <v>360</v>
       </c>
       <c r="S51">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="T51">
         <f t="shared" si="2"/>
-        <v>313</v>
-      </c>
-    </row>
-    <row r="52" spans="3:19" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C52">
         <v>406</v>
       </c>
@@ -5245,11 +5780,15 @@
         <v>365</v>
       </c>
       <c r="S52">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="T52">
         <f t="shared" si="2"/>
-        <v>340</v>
-      </c>
-    </row>
-    <row r="53" spans="3:19" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C53">
         <v>436</v>
       </c>
@@ -5291,11 +5830,15 @@
         <v>374</v>
       </c>
       <c r="S53">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="T53">
         <f t="shared" si="2"/>
-        <v>362</v>
-      </c>
-    </row>
-    <row r="54" spans="3:19" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C54">
         <v>466</v>
       </c>
@@ -5337,11 +5880,15 @@
         <v>425</v>
       </c>
       <c r="S54">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="T54">
         <f t="shared" si="2"/>
-        <v>387</v>
-      </c>
-    </row>
-    <row r="55" spans="3:19" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C55">
         <v>496</v>
       </c>
@@ -5383,11 +5930,15 @@
         <v>484</v>
       </c>
       <c r="S55">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="T55">
         <f t="shared" si="2"/>
-        <v>410</v>
-      </c>
-    </row>
-    <row r="56" spans="3:19" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C56">
         <v>526</v>
       </c>
@@ -5429,11 +5980,15 @@
         <v>459</v>
       </c>
       <c r="S56">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="T56">
         <f t="shared" si="2"/>
-        <v>445</v>
-      </c>
-    </row>
-    <row r="57" spans="3:19" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C57">
         <v>556</v>
       </c>
@@ -5475,11 +6030,15 @@
         <v>524</v>
       </c>
       <c r="S57">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="T57">
         <f t="shared" si="2"/>
-        <v>461</v>
-      </c>
-    </row>
-    <row r="58" spans="3:19" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C58">
         <v>586</v>
       </c>
@@ -5521,11 +6080,15 @@
         <v>530</v>
       </c>
       <c r="S58">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="T58">
         <f t="shared" si="2"/>
-        <v>487</v>
-      </c>
-    </row>
-    <row r="59" spans="3:19" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C59">
         <v>616</v>
       </c>
@@ -5539,7 +6102,7 @@
         <v>543.5</v>
       </c>
     </row>
-    <row r="60" spans="3:19" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C60">
         <v>646</v>
       </c>
@@ -5553,7 +6116,7 @@
         <v>560.29999999999995</v>
       </c>
     </row>
-    <row r="61" spans="3:19" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C61">
         <v>676</v>
       </c>
@@ -5564,6 +6127,1101 @@
         <v>570</v>
       </c>
       <c r="P61">
+        <v>585.20000000000005</v>
+      </c>
+    </row>
+    <row r="62" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B62" t="s">
+        <v>6</v>
+      </c>
+      <c r="C62" t="s">
+        <v>7</v>
+      </c>
+      <c r="D62" t="s">
+        <v>8</v>
+      </c>
+      <c r="E62" t="s">
+        <v>9</v>
+      </c>
+      <c r="F62" t="s">
+        <v>2</v>
+      </c>
+      <c r="G62" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B64">
+        <v>2</v>
+      </c>
+      <c r="C64">
+        <v>2</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+      <c r="F64">
+        <v>1</v>
+      </c>
+      <c r="G64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B65">
+        <v>3</v>
+      </c>
+      <c r="C65">
+        <v>3</v>
+      </c>
+      <c r="D65">
+        <v>3</v>
+      </c>
+      <c r="E65">
+        <v>2</v>
+      </c>
+      <c r="F65">
+        <v>2</v>
+      </c>
+      <c r="G65">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B66">
+        <v>4</v>
+      </c>
+      <c r="C66">
+        <v>4</v>
+      </c>
+      <c r="D66">
+        <v>4</v>
+      </c>
+      <c r="E66">
+        <v>3</v>
+      </c>
+      <c r="F66">
+        <v>3</v>
+      </c>
+      <c r="G66">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B67">
+        <v>5</v>
+      </c>
+      <c r="C67">
+        <v>5</v>
+      </c>
+      <c r="D67">
+        <v>5</v>
+      </c>
+      <c r="E67">
+        <v>4</v>
+      </c>
+      <c r="F67">
+        <v>3</v>
+      </c>
+      <c r="G67">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B68">
+        <v>6</v>
+      </c>
+      <c r="C68">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D68">
+        <v>6</v>
+      </c>
+      <c r="E68">
+        <v>5</v>
+      </c>
+      <c r="F68">
+        <v>3</v>
+      </c>
+      <c r="G68">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B69">
+        <v>7</v>
+      </c>
+      <c r="C69">
+        <v>6.7</v>
+      </c>
+      <c r="D69">
+        <v>7</v>
+      </c>
+      <c r="E69">
+        <v>5</v>
+      </c>
+      <c r="F69">
+        <v>4</v>
+      </c>
+      <c r="G69">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B70">
+        <v>8</v>
+      </c>
+      <c r="C70">
+        <v>7.4</v>
+      </c>
+      <c r="D70">
+        <v>7</v>
+      </c>
+      <c r="E70">
+        <v>6</v>
+      </c>
+      <c r="F70">
+        <v>5</v>
+      </c>
+      <c r="G70">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B71">
+        <v>9</v>
+      </c>
+      <c r="C71">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="D71">
+        <v>9</v>
+      </c>
+      <c r="E71">
+        <v>8</v>
+      </c>
+      <c r="F71">
+        <v>5</v>
+      </c>
+      <c r="G71">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B72">
+        <v>10</v>
+      </c>
+      <c r="C72">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D72">
+        <v>9</v>
+      </c>
+      <c r="E72">
+        <v>8</v>
+      </c>
+      <c r="F72">
+        <v>6</v>
+      </c>
+      <c r="G72">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B73">
+        <v>11</v>
+      </c>
+      <c r="C73">
+        <v>10</v>
+      </c>
+      <c r="D73">
+        <v>11</v>
+      </c>
+      <c r="E73">
+        <v>8</v>
+      </c>
+      <c r="F73">
+        <v>6</v>
+      </c>
+      <c r="G73">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B74">
+        <v>12</v>
+      </c>
+      <c r="C74">
+        <v>11</v>
+      </c>
+      <c r="D74">
+        <v>12</v>
+      </c>
+      <c r="E74">
+        <v>9</v>
+      </c>
+      <c r="F74">
+        <v>6</v>
+      </c>
+      <c r="G74">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B75">
+        <v>13</v>
+      </c>
+      <c r="C75">
+        <v>11.6</v>
+      </c>
+      <c r="D75">
+        <v>12</v>
+      </c>
+      <c r="E75">
+        <v>6</v>
+      </c>
+      <c r="F75">
+        <v>6</v>
+      </c>
+      <c r="G75">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B76">
+        <v>14</v>
+      </c>
+      <c r="C76">
+        <v>11.7</v>
+      </c>
+      <c r="D76">
+        <v>13</v>
+      </c>
+      <c r="E76">
+        <v>12</v>
+      </c>
+      <c r="F76">
+        <v>7</v>
+      </c>
+      <c r="G76">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="77" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B77">
+        <v>15</v>
+      </c>
+      <c r="C77">
+        <v>14.2</v>
+      </c>
+      <c r="D77">
+        <v>14</v>
+      </c>
+      <c r="E77">
+        <v>10</v>
+      </c>
+      <c r="F77">
+        <v>7</v>
+      </c>
+      <c r="G77">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="78" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B78">
+        <v>16</v>
+      </c>
+      <c r="C78">
+        <v>14.5</v>
+      </c>
+      <c r="D78">
+        <v>15</v>
+      </c>
+      <c r="E78">
+        <v>14</v>
+      </c>
+      <c r="F78">
+        <v>8</v>
+      </c>
+      <c r="G78">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="79" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B79">
+        <v>17</v>
+      </c>
+      <c r="C79">
+        <v>14.6</v>
+      </c>
+      <c r="D79">
+        <v>17</v>
+      </c>
+      <c r="E79">
+        <v>15</v>
+      </c>
+      <c r="F79">
+        <v>9</v>
+      </c>
+      <c r="G79">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="80" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B80">
+        <v>18</v>
+      </c>
+      <c r="C80">
+        <v>15.1</v>
+      </c>
+      <c r="D80">
+        <v>18</v>
+      </c>
+      <c r="E80">
+        <v>12</v>
+      </c>
+      <c r="F80">
+        <v>9</v>
+      </c>
+      <c r="G80">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="81" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B81">
+        <v>19</v>
+      </c>
+      <c r="C81">
+        <v>17.2</v>
+      </c>
+      <c r="D81">
+        <v>19</v>
+      </c>
+      <c r="E81">
+        <v>14</v>
+      </c>
+      <c r="F81">
+        <v>10</v>
+      </c>
+      <c r="G81">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="82" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B82">
+        <v>20</v>
+      </c>
+      <c r="C82">
+        <v>16.7</v>
+      </c>
+      <c r="D82">
+        <v>17</v>
+      </c>
+      <c r="E82">
+        <v>15</v>
+      </c>
+      <c r="F82">
+        <v>10</v>
+      </c>
+      <c r="G82">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="83" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B83">
+        <v>21</v>
+      </c>
+      <c r="C83">
+        <v>19</v>
+      </c>
+      <c r="D83">
+        <v>19</v>
+      </c>
+      <c r="E83">
+        <v>16</v>
+      </c>
+      <c r="F83">
+        <v>15</v>
+      </c>
+      <c r="G83">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="84" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B84">
+        <v>26</v>
+      </c>
+      <c r="C84">
+        <v>22.4</v>
+      </c>
+      <c r="D84">
+        <v>23</v>
+      </c>
+      <c r="E84">
+        <v>18</v>
+      </c>
+      <c r="F84">
+        <v>19</v>
+      </c>
+      <c r="G84">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="85" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B85">
+        <v>31</v>
+      </c>
+      <c r="C85">
+        <v>28.4</v>
+      </c>
+      <c r="D85">
+        <v>29</v>
+      </c>
+      <c r="E85">
+        <v>23</v>
+      </c>
+      <c r="F85">
+        <v>23</v>
+      </c>
+      <c r="G85">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="86" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B86">
+        <v>36</v>
+      </c>
+      <c r="C86">
+        <v>33</v>
+      </c>
+      <c r="D86">
+        <v>33</v>
+      </c>
+      <c r="E86">
+        <v>28</v>
+      </c>
+      <c r="F86">
+        <v>28</v>
+      </c>
+      <c r="G86">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="87" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B87">
+        <v>41</v>
+      </c>
+      <c r="C87">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="D87">
+        <v>39</v>
+      </c>
+      <c r="E87">
+        <v>30</v>
+      </c>
+      <c r="F87">
+        <v>30</v>
+      </c>
+      <c r="G87">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="88" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B88">
+        <v>46</v>
+      </c>
+      <c r="C88">
+        <v>42.4</v>
+      </c>
+      <c r="D88">
+        <v>41</v>
+      </c>
+      <c r="E88">
+        <v>35</v>
+      </c>
+      <c r="F88">
+        <v>37</v>
+      </c>
+      <c r="G88">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="89" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B89">
+        <v>51</v>
+      </c>
+      <c r="C89">
+        <v>45.6</v>
+      </c>
+      <c r="D89">
+        <v>44</v>
+      </c>
+      <c r="E89">
+        <v>37</v>
+      </c>
+      <c r="F89">
+        <v>38</v>
+      </c>
+      <c r="G89">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="90" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B90">
+        <v>56</v>
+      </c>
+      <c r="C90">
+        <v>50.8</v>
+      </c>
+      <c r="D90">
+        <v>50</v>
+      </c>
+      <c r="E90">
+        <v>47</v>
+      </c>
+      <c r="F90">
+        <v>41</v>
+      </c>
+      <c r="G90">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="91" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B91">
+        <v>61</v>
+      </c>
+      <c r="C91">
+        <v>54.1</v>
+      </c>
+      <c r="D91">
+        <v>59</v>
+      </c>
+      <c r="E91">
+        <v>49</v>
+      </c>
+      <c r="F91">
+        <v>48</v>
+      </c>
+      <c r="G91">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="92" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B92">
+        <v>66</v>
+      </c>
+      <c r="C92">
+        <v>60.6</v>
+      </c>
+      <c r="D92">
+        <v>62</v>
+      </c>
+      <c r="E92">
+        <v>50</v>
+      </c>
+      <c r="F92">
+        <v>53</v>
+      </c>
+      <c r="G92">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="93" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B93">
+        <v>71</v>
+      </c>
+      <c r="C93">
+        <v>62.8</v>
+      </c>
+      <c r="D93">
+        <v>66</v>
+      </c>
+      <c r="E93">
+        <v>52</v>
+      </c>
+      <c r="F93">
+        <v>56</v>
+      </c>
+      <c r="G93">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="94" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B94">
+        <v>76</v>
+      </c>
+      <c r="C94">
+        <v>67.900000000000006</v>
+      </c>
+      <c r="D94">
+        <v>69</v>
+      </c>
+      <c r="E94">
+        <v>58</v>
+      </c>
+      <c r="F94">
+        <v>58</v>
+      </c>
+      <c r="G94">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="95" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B95">
+        <v>81</v>
+      </c>
+      <c r="C95">
+        <v>76.599999999999994</v>
+      </c>
+      <c r="D95">
+        <v>73</v>
+      </c>
+      <c r="E95">
+        <v>63</v>
+      </c>
+      <c r="F95">
+        <v>65</v>
+      </c>
+      <c r="G95">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="96" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B96">
+        <v>86</v>
+      </c>
+      <c r="C96">
+        <v>77.2</v>
+      </c>
+      <c r="D96">
+        <v>81</v>
+      </c>
+      <c r="E96">
+        <v>63</v>
+      </c>
+      <c r="F96">
+        <v>68</v>
+      </c>
+      <c r="G96">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B97">
+        <v>91</v>
+      </c>
+      <c r="C97">
+        <v>80.7</v>
+      </c>
+      <c r="D97">
+        <v>86</v>
+      </c>
+      <c r="E97">
+        <v>69</v>
+      </c>
+      <c r="F97">
+        <v>73</v>
+      </c>
+      <c r="G97">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="98" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B98">
+        <v>96</v>
+      </c>
+      <c r="C98">
+        <v>82.1</v>
+      </c>
+      <c r="D98">
+        <v>89</v>
+      </c>
+      <c r="E98">
+        <v>76</v>
+      </c>
+      <c r="F98">
+        <v>75</v>
+      </c>
+      <c r="G98">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="99" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B99">
+        <v>101</v>
+      </c>
+      <c r="C99">
+        <v>87.6</v>
+      </c>
+      <c r="D99">
+        <v>90</v>
+      </c>
+      <c r="E99">
+        <v>84</v>
+      </c>
+      <c r="F99">
+        <v>81</v>
+      </c>
+      <c r="G99">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="100" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B100">
+        <v>106</v>
+      </c>
+      <c r="C100">
+        <v>91.6</v>
+      </c>
+      <c r="D100">
+        <v>94</v>
+      </c>
+      <c r="E100">
+        <v>100</v>
+      </c>
+      <c r="F100">
+        <v>82</v>
+      </c>
+      <c r="G100">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="101" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B101">
+        <v>136</v>
+      </c>
+      <c r="C101">
+        <v>116.7</v>
+      </c>
+      <c r="D101">
+        <v>119</v>
+      </c>
+      <c r="E101">
+        <v>118</v>
+      </c>
+      <c r="F101">
+        <v>108</v>
+      </c>
+      <c r="G101">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="102" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B102">
+        <v>166</v>
+      </c>
+      <c r="C102">
+        <v>142.69999999999999</v>
+      </c>
+      <c r="D102">
+        <v>152</v>
+      </c>
+      <c r="E102">
+        <v>144</v>
+      </c>
+      <c r="F102">
+        <v>137</v>
+      </c>
+      <c r="G102">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="103" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B103">
+        <v>196</v>
+      </c>
+      <c r="C103">
+        <v>177.9</v>
+      </c>
+      <c r="D103">
+        <v>179</v>
+      </c>
+      <c r="E103">
+        <v>168</v>
+      </c>
+      <c r="F103">
+        <v>159</v>
+      </c>
+      <c r="G103">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="104" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B104">
+        <v>226</v>
+      </c>
+      <c r="C104">
+        <v>198.7</v>
+      </c>
+      <c r="D104">
+        <v>206</v>
+      </c>
+      <c r="E104">
+        <v>193</v>
+      </c>
+      <c r="F104">
+        <v>183</v>
+      </c>
+      <c r="G104">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="105" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B105">
+        <v>256</v>
+      </c>
+      <c r="C105">
+        <v>226.5</v>
+      </c>
+      <c r="D105">
+        <v>231</v>
+      </c>
+      <c r="E105">
+        <v>237</v>
+      </c>
+      <c r="F105">
+        <v>205</v>
+      </c>
+      <c r="G105">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="106" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B106">
+        <v>286</v>
+      </c>
+      <c r="C106">
+        <v>244.4</v>
+      </c>
+      <c r="D106">
+        <v>260</v>
+      </c>
+      <c r="E106">
+        <v>250</v>
+      </c>
+      <c r="F106">
+        <v>233</v>
+      </c>
+      <c r="G106">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="107" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B107">
+        <v>316</v>
+      </c>
+      <c r="C107">
+        <v>283.3</v>
+      </c>
+      <c r="D107">
+        <v>285</v>
+      </c>
+      <c r="E107">
+        <v>286</v>
+      </c>
+      <c r="F107">
+        <v>263</v>
+      </c>
+      <c r="G107">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="108" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B108">
+        <v>346</v>
+      </c>
+      <c r="C108">
+        <v>295.8</v>
+      </c>
+      <c r="D108">
+        <v>311</v>
+      </c>
+      <c r="E108">
+        <v>316</v>
+      </c>
+      <c r="F108">
+        <v>282</v>
+      </c>
+      <c r="G108">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="109" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B109">
+        <v>376</v>
+      </c>
+      <c r="C109">
+        <v>325.39999999999998</v>
+      </c>
+      <c r="D109">
+        <v>340</v>
+      </c>
+      <c r="E109">
+        <v>360</v>
+      </c>
+      <c r="F109">
+        <v>313</v>
+      </c>
+      <c r="G109">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="110" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B110">
+        <v>406</v>
+      </c>
+      <c r="C110">
+        <v>358.2</v>
+      </c>
+      <c r="D110">
+        <v>369</v>
+      </c>
+      <c r="E110">
+        <v>365</v>
+      </c>
+      <c r="F110">
+        <v>340</v>
+      </c>
+      <c r="G110">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="111" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B111">
+        <v>436</v>
+      </c>
+      <c r="C111">
+        <v>376.9</v>
+      </c>
+      <c r="D111">
+        <v>397</v>
+      </c>
+      <c r="E111">
+        <v>374</v>
+      </c>
+      <c r="F111">
+        <v>362</v>
+      </c>
+      <c r="G111">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="112" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B112">
+        <v>466</v>
+      </c>
+      <c r="C112">
+        <v>403.4</v>
+      </c>
+      <c r="D112">
+        <v>430</v>
+      </c>
+      <c r="E112">
+        <v>425</v>
+      </c>
+      <c r="F112">
+        <v>387</v>
+      </c>
+      <c r="G112">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="113" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B113">
+        <v>496</v>
+      </c>
+      <c r="C113">
+        <v>424</v>
+      </c>
+      <c r="D113">
+        <v>456</v>
+      </c>
+      <c r="E113">
+        <v>484</v>
+      </c>
+      <c r="F113">
+        <v>410</v>
+      </c>
+      <c r="G113">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="114" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B114">
+        <v>526</v>
+      </c>
+      <c r="C114">
+        <v>460.5</v>
+      </c>
+      <c r="D114">
+        <v>472</v>
+      </c>
+      <c r="E114">
+        <v>459</v>
+      </c>
+      <c r="F114">
+        <v>445</v>
+      </c>
+      <c r="G114">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="115" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B115">
+        <v>556</v>
+      </c>
+      <c r="C115">
+        <v>480.9</v>
+      </c>
+      <c r="D115">
+        <v>502</v>
+      </c>
+      <c r="E115">
+        <v>524</v>
+      </c>
+      <c r="F115">
+        <v>461</v>
+      </c>
+      <c r="G115">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="116" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B116">
+        <v>586</v>
+      </c>
+      <c r="C116">
+        <v>516.9</v>
+      </c>
+      <c r="D116">
+        <v>534</v>
+      </c>
+      <c r="E116">
+        <v>530</v>
+      </c>
+      <c r="F116">
+        <v>487</v>
+      </c>
+      <c r="G116">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="117" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C117">
+        <v>543.5</v>
+      </c>
+    </row>
+    <row r="118" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C118">
+        <v>560.29999999999995</v>
+      </c>
+    </row>
+    <row r="119" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C119">
         <v>585.20000000000005</v>
       </c>
     </row>

</xml_diff>